<commit_message>
Actualizar scripts de DBeaver
</commit_message>
<xml_diff>
--- a/7otros_CGE/SISPOA CONAUD/SISPOA/REPORTES/REPORTE EXCEL/Reporte 1/reporte para CONAUD.xlsx
+++ b/7otros_CGE/SISPOA CONAUD/SISPOA/REPORTES/REPORTE EXCEL/Reporte 1/reporte para CONAUD.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="189">
   <si>
     <t xml:space="preserve">Detalle de Auditorias/Seguimiento/Supervisiones/Confiabilidad - En ejecución</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">Tipo de Auditoria</t>
   </si>
   <si>
+    <t xml:space="preserve">Estado CONAUD</t>
+  </si>
+  <si>
     <t xml:space="preserve">500.1201.44.1.24</t>
   </si>
   <si>
@@ -64,6 +67,9 @@
     <t xml:space="preserve">AUDITORÍA</t>
   </si>
   <si>
+    <t xml:space="preserve">NO INICIADA EN CONAUD</t>
+  </si>
+  <si>
     <t xml:space="preserve">500.1201.46.1.24</t>
   </si>
   <si>
@@ -85,12 +91,15 @@
     <t xml:space="preserve">GOBIERNO AUTÓNOMO DEPARTAMENTAL DE LA PAZ</t>
   </si>
   <si>
-    <t xml:space="preserve">EVALUAR SI LOS INFORMES DE AUDITORIA DE CONBIALIDAD DE REGISTROS Y ESTADOS FINANCIEROS, EMITIDOS POR LA UNIDAD DE </t>
+    <t xml:space="preserve">EVALUAR SI LOS INFORMES DE AUDITORIA DE CONBIALIDAD DE REGISTROS Y ESTADOS FINANCIEROS, EMITIDOS POR LA UNIDAD DE AUDITORIA INTERNA, SE AJUSTAN A LAS NORMAS DE AUDITORIA DE CONFIABILIDAD DE REGISTROS Y ESTADOS FINANCIEROS</t>
   </si>
   <si>
     <t xml:space="preserve">CONFIABILIDAD</t>
   </si>
   <si>
+    <t xml:space="preserve">CONSOLIDADO</t>
+  </si>
+  <si>
     <t xml:space="preserve">510.1201.16.2.24</t>
   </si>
   <si>
@@ -106,9 +115,15 @@
     <t xml:space="preserve">SERVICIO DEPARTAMENTAL DE SALUD LA PAZ</t>
   </si>
   <si>
+    <t xml:space="preserve">HISTORICO</t>
+  </si>
+  <si>
     <t xml:space="preserve">520.1201.48.2.24</t>
   </si>
   <si>
+    <t xml:space="preserve">EDICION</t>
+  </si>
+  <si>
     <t xml:space="preserve">520.1201.48.3.24</t>
   </si>
   <si>
@@ -118,19 +133,19 @@
     <t xml:space="preserve">520.1201.49.1.24</t>
   </si>
   <si>
-    <t xml:space="preserve">EMITIR UNA OPINIÓN INDEPENDIENTE SOBRE EL CUMPLIMIENTO DEL ORDENAMIENTO JURÍDICO Y DISPOSICIONES LEGALES EN LA </t>
+    <t xml:space="preserve">EMITIR UNA OPINIÓN INDEPENDIENTE SOBRE EL CUMPLIMIENTO DEL ORDENAMIENTO JURÍDICO Y DISPOSICIONES LEGALES EN LA DESVINCULACIÓN DEL PERSONAL DE PROMES, POR LOS MESES DE ENERO, FEBRERO Y MARZO DE 2021</t>
   </si>
   <si>
     <t xml:space="preserve">520.1201.49.2.24</t>
   </si>
   <si>
-    <t xml:space="preserve">EMITIR UN PRONUNCIAMIENTO SOBRE EL CUMPLIMIENTO DEL ORDENAMIENTO JURÍDICO ADMINISTRATIVO Y OTRAS NORMAS LEGALES </t>
+    <t xml:space="preserve">EMITIR UN PRONUNCIAMIENTO SOBRE EL CUMPLIMIENTO DEL ORDENAMIENTO JURÍDICO ADMINISTRATIVO Y OTRAS NORMAS LEGALES APLICABLES Y OBLIGACIONES CONTRACTUALES EN LA CONSTRUCCIÓN DEL PROYECTO</t>
   </si>
   <si>
     <t xml:space="preserve">520.1201.49.3.24</t>
   </si>
   <si>
-    <t xml:space="preserve">EMITIR UN PRONUNCIAMIENTO SOBRE EL CUMPLIMIENTO DEL ORDENAMIENTO JURÍDICO ADMINISTRATIVO Y OTRAS NORMAS APLICABLES </t>
+    <t xml:space="preserve">EMITIR UN PRONUNCIAMIENTO SOBRE EL CUMPLIMIENTO DEL ORDENAMIENTO JURÍDICO ADMINISTRATIVO Y OTRAS NORMAS APLICABLES Y OBLIGACIONES CONTRACTULAES EN LA CONSTRUCCIÓN DEL PROYECTO  DE "IMPLEMENTACIÓN Y APLICACIÓN DE LA PLANTA PROCESADORA DE CEREALES"</t>
   </si>
   <si>
     <t xml:space="preserve">520.1201.50.1.24</t>
@@ -178,7 +193,7 @@
     <t xml:space="preserve">COMITÉ EJECUTIVO DE LA UNIVERSIDAD BOLIVIANA</t>
   </si>
   <si>
-    <t xml:space="preserve">EVALUAR SI LOS INFORMES DE AUDITORIA DE CONFIABILIDAD DE REGISTROS Y ESTADOS FINANCIEROS, EMITIDOS POR LA UNIDAD DE </t>
+    <t xml:space="preserve">EVALUAR SI LOS INFORMES DE AUDITORIA DE CONFIABILIDAD DE REGISTROS Y ESTADOS FINANCIEROS, EMITIDOS POR LA UNIDAD DE AUDITORIA INTERNA, SE AJUSTAN A LAS NORMAS DE AUDITORIA DE CONFIABILIDAD DE REGISTROS Y ESTADOS FINANCIEROS</t>
   </si>
   <si>
     <t xml:space="preserve">510.1201.16.5.24</t>
@@ -190,7 +205,7 @@
     <t xml:space="preserve">510.1201.16.6.24</t>
   </si>
   <si>
-    <t xml:space="preserve">UNIVERSIDAD INDÍGENA BOLIVIANA COMUNITARIA INTERCULTURAL PRODUCTIVA </t>
+    <t xml:space="preserve">UNIVERSIDAD INDÍGENA BOLIVIANA COMUNITARIA INTERCULTURAL PRODUCTIVA TUPAK KATARI</t>
   </si>
   <si>
     <t xml:space="preserve">510.1201.16.7.24</t>
@@ -199,7 +214,7 @@
     <t xml:space="preserve">UNIVERSIDAD MAYOR DE SAN ANDRÉS</t>
   </si>
   <si>
-    <t xml:space="preserve">EVALUAR SI LOS INFORMES DE AUDITORÍA DE CONFIABILIDAD DE REGISTROS Y ESTADOS FINANIEROS, EMITIDOS POR LA UNIDAD DE </t>
+    <t xml:space="preserve">EVALUAR SI LOS INFORMES DE AUDITORÍA DE CONFIABILIDAD DE REGISTROS Y ESTADOS FINANIEROS, EMITIDOS POR LA UNIDAD DE AUDITORÍA INTERNA, SE AJUSTAN A LAS NORMAS DE AUDITORÍA DE CONFIABILIDAD DE REGISTROS Y ESTADOS FINANCIEROS</t>
   </si>
   <si>
     <t xml:space="preserve">510.1201.16.8.24</t>
@@ -208,19 +223,19 @@
     <t xml:space="preserve">SERVICIO DEPARTAMENTAL DE RIEGO - LA PAZ</t>
   </si>
   <si>
-    <t xml:space="preserve">EVALUAR SI LOS INFORMES DE AUDITORIA DE CONFIABILIDAD DE RESGISTROS Y ESTADOS FINANCIDEROS, EMITIDOS, SE AJUSTAN A LAS </t>
+    <t xml:space="preserve">EVALUAR SI LOS INFORMES DE AUDITORIA DE CONFIABILIDAD DE RESGISTROS Y ESTADOS FINANCIDEROS, EMITIDOS, SE AJUSTAN A LAS NORMAS DE AUDITORIA DE CONFIABILIDAD DE REGISTROS Y ESTADOS FINANCIEROS</t>
   </si>
   <si>
     <t xml:space="preserve">520.1201.269.1.24</t>
   </si>
   <si>
-    <t xml:space="preserve">EMITIR OPINIÓN INDEPENDIENTE SOBRE EL ORDENAMIENTO JURÍDICO ADMINISTRATIVO DE LOS PAGOS EFECTUADOS Y PAGOS </t>
+    <t xml:space="preserve">EMITIR OPINIÓN INDEPENDIENTE SOBRE EL ORDENAMIENTO JURÍDICO ADMINISTRATIVO DE LOS PAGOS EFECTUADOS Y PAGOS PENDIENTES  DE LA EJECUCIÓN DEL CONTRATO DE OBRA N° LPN/55/2017</t>
   </si>
   <si>
     <t xml:space="preserve">520.1201.48.5.24</t>
   </si>
   <si>
-    <t xml:space="preserve">EMITIR OPINIÓN INDEPENDIENTE SOBRE EL CUMPLIMIENTO DEL ORDENAMIENTOS JURIDICO ADMINISTRATIVO DEL PROCESO DE </t>
+    <t xml:space="preserve">EMITIR OPINIÓN INDEPENDIENTE SOBRE EL CUMPLIMIENTO DEL ORDENAMIENTOS JURIDICO ADMINISTRATIVO DEL PROCESO DE CONTRATACIÓN Y PAGO DEL SERVICIOS DE AUDITORIA DE CONFIABILIDAD DE REGISTROS Y ESTADOS FINANCIEROS 2022 DEL SEDERI LA PAZ</t>
   </si>
   <si>
     <t xml:space="preserve">520.1202.54.9.24</t>
@@ -235,6 +250,9 @@
     <t xml:space="preserve">Verificar el cumplimiento de las disposiciones legales en los procesos de contratación menor.</t>
   </si>
   <si>
+    <t xml:space="preserve">VERIFICADO</t>
+  </si>
+  <si>
     <t xml:space="preserve">520.1202.54.7.24</t>
   </si>
   <si>
@@ -367,7 +385,7 @@
     <t xml:space="preserve">520.1202.56.4.24</t>
   </si>
   <si>
-    <t xml:space="preserve">EMITIR OPINIÓN INDEPENDIENTE SOBRE EL CUMPLIMIENTO DEL OBJETO Y CLÁUSULAS RELACIONADAS DEL CONTRATO OF N° 02/2022 </t>
+    <t xml:space="preserve">EMITIR OPINIÓN INDEPENDIENTE SOBRE EL CUMPLIMIENTO DEL OBJETO Y CLÁUSULAS RELACIONADAS DEL CONTRATO OF N° 02/2022 “CONTRATO ADMINISTRATIVO PARA LA PRESTACIÓN DEL SERVICIO DE CONSULTORÍA: AUDITORÍA DE PROYECTOS DE INVERSIÓN PÚBLICA DE PROYECTOS FINANCIADOS POR LA UNIDAD DE PROYECTOS ESPECIALES (UPRE) DEL GAM CAJUATA”, CONSIDERANDO LAS NORMAS DE AUDITORÍA DE PROYECTOS DE INVERSIÓN PÚBLICA</t>
   </si>
   <si>
     <t xml:space="preserve">510.1202.17.14.24</t>
@@ -376,7 +394,7 @@
     <t xml:space="preserve">GOBIERNO AUTÓNOMO MUNICIPAL DE PUCARANI</t>
   </si>
   <si>
-    <t xml:space="preserve">ESTABLECER SI LOS INFORMES DE AUDITORIA INTERNA NRS GAMP/UAI/AUCONF-01/2024 Y GAMP/UAI/AUCONF-02/2024, FUERON EMITIDOS </t>
+    <t xml:space="preserve">ESTABLECER SI LOS INFORMES DE AUDITORIA INTERNA NRS GAMP/UAI/AUCONF-01/2024 Y GAMP/UAI/AUCONF-02/2024, FUERON EMITIDOS APLICANDO LAS NORMAS DE CONFIABILIDAD DE LOS REGISTROS Y ESTADOS FINANCIEROS Y LAS NORMAS GENERALES DE AUDITORIA GUBERNAMENTAL.</t>
   </si>
   <si>
     <t xml:space="preserve">520.1202.54.10.24</t>
@@ -385,13 +403,13 @@
     <t xml:space="preserve">GOBIERNO AUTÓNOMO MUNICIPAL DE PATACAMAYA</t>
   </si>
   <si>
-    <t xml:space="preserve">EMITIR UNA OPINIÓN INDEPENDIENTE SOBRE EL CUMPLIMIENTO DEL ORDENAMIENTO JURÍDICO ADMINISTRATIVO Y NORMAS LEGALES </t>
+    <t xml:space="preserve">EMITIR UNA OPINIÓN INDEPENDIENTE SOBRE EL CUMPLIMIENTO DEL ORDENAMIENTO JURÍDICO ADMINISTRATIVO Y NORMAS LEGALES APLICABLES SOBRE "CUENTAS POR COBRAR", ORIGINADOS EN DESEMBOLSOS DE RECURSOS REGISTRADOS DE LA CUENTA FONDOS EN AVANCE.</t>
   </si>
   <si>
     <t xml:space="preserve">520.1202.56.5.24</t>
   </si>
   <si>
-    <t xml:space="preserve">EMITIR OPINIÓN INDEPENDIENTE. SOBRE EL CUMPLIMIENTO DEL OBJETO Y CLÁUSULAS RELACIONADAS DE LA MINUTA DE CONTRATO </t>
+    <t xml:space="preserve">EMITIR OPINIÓN INDEPENDIENTE. SOBRE EL CUMPLIMIENTO DEL OBJETO Y CLÁUSULAS RELACIONADAS DE LA MINUTA DE CONTRATO GAMV/CA/N°022/2011 DEL 22/02/2021, PARA PRESTAR EL SERVICIO DE “AUDITORÍA OPERATIVA - SECCIONAL - GESTIÓN 2020, SUSCRITA EL 22 DE FECBRERO DE 2021, ENTRE EL GAM VIACHA Y LA FIRMA DE AUDITORÍA “GUTIÉRREZ &amp; THOMPSON ASOCIADOS S.R.L. - G&amp;T”.</t>
   </si>
   <si>
     <t xml:space="preserve">500.1202.51.1.24</t>
@@ -457,7 +475,7 @@
     <t xml:space="preserve">520.1203.53.8.24</t>
   </si>
   <si>
-    <t xml:space="preserve">EMITIR UNA OPINIÓN INDEPENDIENTE SOBRE EL CUMPLIMIENTO DE DISPOSICIONES LEGALES RELACIONADAS CON EL DESEMBOLSO DE </t>
+    <t xml:space="preserve">EMITIR UNA OPINIÓN INDEPENDIENTE SOBRE EL CUMPLIMIENTO DE DISPOSICIONES LEGALES RELACIONADAS CON EL DESEMBOLSO DE RECURSOS MEDIANTE CHEQUES (CASOS ESPECÍFICOS)</t>
   </si>
   <si>
     <t xml:space="preserve">520.1202.53.6.24</t>
@@ -496,7 +514,7 @@
     <t xml:space="preserve">520.1203.53.9.24</t>
   </si>
   <si>
-    <t xml:space="preserve">EMITIR UNA OPINIÓN INDEPENDIENTE SOBRE EL CUMPLIMIENTO DEL ORDENAMIENTO JURÍDICO ADMINISTRATIVO Y CUMPLIMIENTO DE LOS </t>
+    <t xml:space="preserve">EMITIR UNA OPINIÓN INDEPENDIENTE SOBRE EL CUMPLIMIENTO DEL ORDENAMIENTO JURÍDICO ADMINISTRATIVO Y CUMPLIMIENTO DE LOS OBJETIVOS DEL PROYECTO CONSTRUCCIÓN SISTEMA DE RIEGO MARKA VILLA EXALTACIÓN.</t>
   </si>
   <si>
     <t xml:space="preserve">520.1202.57.1.24</t>
@@ -508,7 +526,7 @@
     <t xml:space="preserve">520.1203.53.10.24</t>
   </si>
   <si>
-    <t xml:space="preserve">EMITIR UNA OPINIÓN INDEPENDIENTE SOBRE EL CUMPLIMIENTO DE DISPOSICIONES LEGALES APLICABLES Y CUMPLIMIENTO DE LOS </t>
+    <t xml:space="preserve">EMITIR UNA OPINIÓN INDEPENDIENTE SOBRE EL CUMPLIMIENTO DE DISPOSICIONES LEGALES APLICABLES Y CUMPLIMIENTO DE LOS OBJETIVOS DEL PROYECTO CONSTRUCCIÓN CURVAS NORTE –SUR ESTADIUM ANDINO COSMOS 79 (FASE 1)</t>
   </si>
   <si>
     <t xml:space="preserve">520.1202.53.2.24</t>
@@ -581,7 +599,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -626,6 +644,48 @@
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="5.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="6.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="4"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -687,7 +747,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -705,6 +765,30 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -827,7 +911,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:H91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -839,9 +923,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="71.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="117.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="37.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="67.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="96.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="35.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -854,6 +939,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
@@ -865,6 +951,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -886,26 +973,32 @@
       <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="H3" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -913,20 +1006,23 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -934,20 +1030,23 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -955,20 +1054,23 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -976,20 +1078,23 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -997,20 +1102,23 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1018,20 +1126,23 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1039,20 +1150,23 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1060,20 +1174,23 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1081,20 +1198,23 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1102,20 +1222,23 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1123,20 +1246,23 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>33</v>
+        <v>21</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1144,20 +1270,23 @@
         <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>35</v>
+        <v>21</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1165,20 +1294,23 @@
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1186,20 +1318,23 @@
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1207,20 +1342,23 @@
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1228,20 +1366,23 @@
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1249,20 +1390,23 @@
         <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1270,20 +1414,23 @@
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>43</v>
+        <v>21</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>44</v>
+        <v>49</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1291,20 +1438,23 @@
         <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>44</v>
+        <v>49</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1312,20 +1462,23 @@
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1333,20 +1486,23 @@
         <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1354,20 +1510,23 @@
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>51</v>
+        <v>55</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1375,20 +1534,23 @@
         <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>51</v>
+        <v>58</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1396,20 +1558,23 @@
         <v>25</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1417,20 +1582,23 @@
         <v>26</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1438,20 +1606,23 @@
         <v>27</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1459,20 +1630,23 @@
         <v>28</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>63</v>
+        <v>21</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1480,20 +1654,23 @@
         <v>29</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F32" s="4" t="s">
         <v>65</v>
       </c>
+      <c r="F32" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="G32" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1501,20 +1678,23 @@
         <v>30</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1522,20 +1702,23 @@
         <v>31</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1543,20 +1726,23 @@
         <v>32</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1564,20 +1750,23 @@
         <v>33</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1585,20 +1774,23 @@
         <v>34</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1606,20 +1798,23 @@
         <v>35</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1627,20 +1822,23 @@
         <v>36</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1648,20 +1846,23 @@
         <v>37</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1669,20 +1870,23 @@
         <v>38</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1690,20 +1894,23 @@
         <v>39</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1711,20 +1918,23 @@
         <v>40</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1732,20 +1942,23 @@
         <v>41</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1753,20 +1966,23 @@
         <v>42</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1774,20 +1990,23 @@
         <v>43</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>97</v>
+        <v>16</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1795,20 +2014,23 @@
         <v>44</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1816,20 +2038,23 @@
         <v>45</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>102</v>
+        <v>16</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1837,20 +2062,23 @@
         <v>46</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>104</v>
+        <v>16</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1858,20 +2086,23 @@
         <v>47</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1879,20 +2110,23 @@
         <v>48</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1900,20 +2134,23 @@
         <v>49</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1921,20 +2158,23 @@
         <v>50</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1942,20 +2182,23 @@
         <v>51</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>114</v>
+        <v>88</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>120</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1963,20 +2206,23 @@
         <v>52</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>117</v>
+        <v>122</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1984,20 +2230,23 @@
         <v>53</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2005,20 +2254,23 @@
         <v>54</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>122</v>
+        <v>86</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2026,20 +2278,23 @@
         <v>55</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2047,20 +2302,23 @@
         <v>56</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2068,20 +2326,23 @@
         <v>57</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2089,20 +2350,23 @@
         <v>58</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2110,20 +2374,23 @@
         <v>59</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2131,20 +2398,23 @@
         <v>60</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2152,20 +2422,23 @@
         <v>61</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2173,20 +2446,23 @@
         <v>62</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E65" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F65" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F65" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="G65" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2194,20 +2470,23 @@
         <v>63</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2215,20 +2494,23 @@
         <v>64</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2236,20 +2518,23 @@
         <v>65</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>144</v>
+        <v>84</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>150</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2257,20 +2542,23 @@
         <v>66</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2278,20 +2566,23 @@
         <v>67</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2299,20 +2590,23 @@
         <v>68</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2320,20 +2614,23 @@
         <v>69</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2341,20 +2638,23 @@
         <v>70</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2362,20 +2662,23 @@
         <v>71</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C74" s="4"/>
       <c r="D74" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>157</v>
+        <v>145</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>163</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2383,20 +2686,23 @@
         <v>72</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C75" s="4"/>
       <c r="D75" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2404,20 +2710,23 @@
         <v>73</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F76" s="4" t="s">
-        <v>161</v>
+        <v>135</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>167</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2425,20 +2734,23 @@
         <v>74</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2446,20 +2758,23 @@
         <v>75</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2467,20 +2782,23 @@
         <v>76</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C79" s="4"/>
       <c r="D79" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2488,20 +2806,23 @@
         <v>77</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2509,20 +2830,23 @@
         <v>78</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2530,20 +2854,23 @@
         <v>79</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C82" s="4"/>
       <c r="D82" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2551,20 +2878,23 @@
         <v>80</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H83" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2572,20 +2902,23 @@
         <v>81</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F84" s="4" t="s">
-        <v>97</v>
+        <v>16</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2593,20 +2926,23 @@
         <v>82</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C85" s="4"/>
       <c r="D85" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F85" s="4" t="s">
-        <v>102</v>
+        <v>16</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2614,20 +2950,23 @@
         <v>83</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C86" s="4"/>
       <c r="D86" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>104</v>
+        <v>16</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2635,20 +2974,23 @@
         <v>84</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C87" s="4"/>
       <c r="D87" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2656,20 +2998,23 @@
         <v>85</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C88" s="4"/>
       <c r="D88" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2677,20 +3022,23 @@
         <v>86</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C89" s="4"/>
       <c r="D89" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2698,20 +3046,23 @@
         <v>87</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C90" s="4"/>
       <c r="D90" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="G90" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2719,27 +3070,30 @@
         <v>88</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C91" s="4"/>
       <c r="D91" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="92">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D2:H2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>

</xml_diff>